<commit_message>
Fired logic and interface
</commit_message>
<xml_diff>
--- a/Documents/Доработки.xlsx
+++ b/Documents/Доработки.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="11835"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28740" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Текущи" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
   <si>
     <t>Текущи корекции</t>
   </si>
@@ -196,22 +196,7 @@
     <t>Изчисляването на празниците за нощна смяна да става съобразно правилата за застъпване и часовия пояс.</t>
   </si>
   <si>
-    <t>При единичен прогнозен график да се добави рекапитулация</t>
-  </si>
-  <si>
     <t>Да се създадат типове на звената</t>
-  </si>
-  <si>
-    <t>Да се оставят само първите 6 реда от рекапитулацията</t>
-  </si>
-  <si>
-    <t>Да се добави ред допълнителни преди реда общо</t>
-  </si>
-  <si>
-    <t>Да се добави ред общо</t>
-  </si>
-  <si>
-    <t>Хората които дават дежурство и са неекипирани да се появяват в разпечатката.</t>
   </si>
   <si>
     <t>Рекапитуалиция по типове звена 
@@ -588,10 +573,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,12 +738,12 @@
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="8"/>
@@ -766,7 +751,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>58</v>
@@ -776,87 +761,32 @@
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>59</v>
-      </c>
+      <c r="B15" s="13"/>
       <c r="C15" s="5"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="13"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="9" t="s">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="12" t="s">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E18" s="2">
         <v>42461</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="12" t="s">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="12" t="s">
-        <v>64</v>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1370,7 +1300,7 @@
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>